<commit_message>
Sprint 3 Documentation Upload
Completed items for Sprint 3
</commit_message>
<xml_diff>
--- a/Michael/Efforts Logbook.xlsx
+++ b/Michael/Efforts Logbook.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -45,24 +45,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Powerpoint</t>
-  </si>
-  <si>
-    <t>Sprint2.ppt</t>
-  </si>
-  <si>
-    <t>Slide 4 to 6</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Someclass.java</t>
-  </si>
-  <si>
-    <t>New code(20), Updated(3)</t>
-  </si>
-  <si>
     <t>Project plan</t>
   </si>
   <si>
@@ -225,9 +207,6 @@
     <t>Project 13</t>
   </si>
   <si>
-    <t>Sprint # 0</t>
-  </si>
-  <si>
     <t>Wrote the Project Plan for the original sprint, as well as a rough guideline for the rest of the sprints (no future tasks added), made 1 - 4 on risk analysis, created GitHub for project with most of the branches and a simple read me, and added information to the PowerPoint.</t>
   </si>
   <si>
@@ -249,9 +228,6 @@
     <t>ProjectPlan, RiskAnalysisSprint2, BestStandards&amp;Practices, Security and Ethical Concerns, (Socio-Economical, Biz Objectives, and Gap Analysis)</t>
   </si>
   <si>
-    <t>ProjectPlan.mpp, RiskAnalysisSprint2, BestStandards&amp;Practices.docx, Security and Ethical Concerns.docx, (Socio-Economical, Biz Objectives, and Gap Analysis.docx)</t>
-  </si>
-  <si>
     <t>All of the project plan and risk analysis for Sprint 2, as well as all of the previously mentioned documentation,  Slides 12, 14, 15</t>
   </si>
   <si>
@@ -259,6 +235,21 @@
   </si>
   <si>
     <t>B, D, E, F, G, K, L, M, N</t>
+  </si>
+  <si>
+    <t>Wrote the Project Plan for Sprint 3, did the risk analysis for Sprint 3, wrote the documentation for Hardware Requirements, Non-Functional Requirments, Persistant Data Storage, and Network Protocol</t>
+  </si>
+  <si>
+    <t>ProjectPlan, RiskAnalysisSprint3, Hardware Requirements, NonFunctional Requirements, Persistant Data Storage, Network Protocol</t>
+  </si>
+  <si>
+    <t>ProjectPlan.mpp, RiskAnalysisSprint2.xlsx, BestStandards&amp;Practices.docx, Security and Ethical Concerns.docx, (Socio-Economical, Biz Objectives, and Gap Analysis.docx)</t>
+  </si>
+  <si>
+    <t>ProjectPlan.mpp, RiskAnalysisSprint3.xlsx, Hardware Requirements.doc, NonFunctional Requirements.doc, Persistant Data Storage.doc, Network Protocol.doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All of the project plan and risk analysis for Sprint 2, as well as all of the previously mentioned documentation,  Slides </t>
   </si>
 </sst>
 </file>
@@ -302,6 +293,7 @@
       <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -415,44 +407,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -468,18 +466,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -491,6 +477,24 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -791,301 +795,288 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="A1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="20" t="s">
+      <c r="A2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>25</v>
+      <c r="A3" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="27">
+        <v>10</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="29">
+        <v>16</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="6">
+      <c r="G5" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="29">
+        <v>16</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="7">
-        <v>16</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
+  <mergeCells count="17">
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1110,328 +1101,328 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
+      <c r="A1" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="17"/>
+      <c r="A2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="G4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="J4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="8" t="s">
+      <c r="M4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="N4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="O4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="P4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+    </row>
+    <row r="5" spans="1:16" s="3" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>0</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="10">
+      <c r="B5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="8">
         <v>2</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>3</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>1</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>1</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <v>5</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="8">
         <v>2</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>3</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="8">
         <v>2</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="8">
         <v>6</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="8">
         <v>3</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="8">
         <v>1</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="8">
         <v>1</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="8">
         <v>5</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>1</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>2</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <v>4</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="7">
         <v>8</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>